<commit_message>
Update doc design UI
</commit_message>
<xml_diff>
--- a/shared/2.2 UI/QLYTHUEXE-tailieuthietke/TaiLieuThietKeChiTiet/QLYTHUEXE_TLPT_01_SignIn.xlsx
+++ b/shared/2.2 UI/QLYTHUEXE-tailieuthietke/TaiLieuThietKeChiTiet/QLYTHUEXE_TLPT_01_SignIn.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10917"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr saveExternalLinkValues="0" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phamquocvy/Downloads/QLYTHUEXE-tailieuthietke/TaiLieuThietKeChiTiet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\QLYTHUEXE-tailieuthietke\QLYTHUEXE-tailieuthietke\TaiLieuThietKeChiTiet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E2F7E63-53F2-C14F-AD04-6E1CC3435F95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="20040" tabRatio="826" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="504" windowWidth="38400" windowHeight="20040" tabRatio="826" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Trang_bìa" sheetId="19" r:id="rId1"/>
@@ -677,15 +676,6 @@
     <t>Truy xuất</t>
   </si>
   <si>
-    <t>a. Truy vấn Firebase Authentication qua đối tượng của lớp FirebaseAuth</t>
-  </si>
-  <si>
-    <t>Câu truy vấn: FirebaseAuth.signInWithEmailAndPassword(email, password)</t>
-  </si>
-  <si>
-    <t>- Nếu thành công: lưu user và chuyển vào màn hình chính</t>
-  </si>
-  <si>
     <t>- Nếu thất bại: thông báo tại màn hình này</t>
   </si>
   <si>
@@ -708,9 +698,6 @@
   </si>
   <si>
     <t>LOGIN_SUCCESS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kiểm tra lại email và password </t>
   </si>
   <si>
     <t xml:space="preserve">Đăng nhập thành công </t>
@@ -791,11 +778,23 @@
   <si>
     <t>Table quản lý user</t>
   </si>
+  <si>
+    <t xml:space="preserve">a. Truy vấn CSDL qua AuthService </t>
+  </si>
+  <si>
+    <t>Câu truy vấn: AuthService.loginAsync(UserName, Password)</t>
+  </si>
+  <si>
+    <t>- Nếu thành công: lưu thông tin customer và chuyển vào màn hình chính</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kiểm tra lại username và password </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;;@"/>
     <numFmt numFmtId="165" formatCode="yyyy/mm/dd;@"/>
@@ -3031,9 +3030,9 @@
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="標準_AP生産依頼 回答リスト画面" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="標準_基本要件仕様書_20061109" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="標準_基本設計書(FWIH105)" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="標準_AP生産依頼 回答リスト画面" xfId="1"/>
+    <cellStyle name="標準_基本要件仕様書_20061109" xfId="3"/>
+    <cellStyle name="標準_基本設計書(FWIH105)" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -17377,9 +17376,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>101600</xdr:colOff>
+          <xdr:colOff>99060</xdr:colOff>
           <xdr:row>1</xdr:row>
-          <xdr:rowOff>165100</xdr:rowOff>
+          <xdr:rowOff>167640</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -17812,22 +17811,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:AX161"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A42" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A152" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="BG116" sqref="BG116"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13.5" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" customHeight="1"/>
   <cols>
     <col min="1" max="49" width="2.6640625" style="20" customWidth="1"/>
-    <col min="50" max="59" width="3.1640625" style="20" customWidth="1"/>
+    <col min="50" max="59" width="3.109375" style="20" customWidth="1"/>
     <col min="60" max="16384" width="9" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" s="19" customFormat="1" ht="17" customHeight="1" thickTop="1">
+    <row r="1" spans="1:49" s="19" customFormat="1" ht="16.95" customHeight="1" thickTop="1">
       <c r="A1" s="215" t="s">
         <v>97</v>
       </c>
@@ -17863,7 +17862,7 @@
       <c r="Y1" s="232"/>
       <c r="Z1" s="233"/>
       <c r="AA1" s="237" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="AB1" s="216"/>
       <c r="AC1" s="216"/>
@@ -17892,7 +17891,7 @@
       <c r="AV1" s="269"/>
       <c r="AW1" s="270"/>
     </row>
-    <row r="2" spans="1:49" s="19" customFormat="1" ht="17" customHeight="1">
+    <row r="2" spans="1:49" s="19" customFormat="1" ht="16.95" customHeight="1">
       <c r="A2" s="218"/>
       <c r="B2" s="219"/>
       <c r="C2" s="219"/>
@@ -17947,7 +17946,7 @@
       <c r="AV2" s="266"/>
       <c r="AW2" s="267"/>
     </row>
-    <row r="3" spans="1:49" ht="17" customHeight="1" thickBot="1">
+    <row r="3" spans="1:49" ht="16.95" customHeight="1" thickBot="1">
       <c r="A3" s="221"/>
       <c r="B3" s="222"/>
       <c r="C3" s="222"/>
@@ -17977,7 +17976,7 @@
       <c r="Y3" s="229"/>
       <c r="Z3" s="230"/>
       <c r="AA3" s="225" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="AB3" s="226"/>
       <c r="AC3" s="226"/>
@@ -17993,7 +17992,7 @@
       <c r="AK3" s="254"/>
       <c r="AL3" s="255"/>
       <c r="AM3" s="225" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="AN3" s="226"/>
       <c r="AO3" s="226"/>
@@ -18233,7 +18232,7 @@
     <row r="13" spans="1:49" ht="13.5" customHeight="1">
       <c r="A13" s="21"/>
       <c r="B13" s="271" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C13" s="272"/>
       <c r="D13" s="272"/>
@@ -19273,7 +19272,7 @@
       <c r="AV40" s="26"/>
       <c r="AW40" s="183"/>
     </row>
-    <row r="41" spans="1:49" s="19" customFormat="1" ht="17" customHeight="1" thickTop="1">
+    <row r="41" spans="1:49" s="19" customFormat="1" ht="16.95" customHeight="1" thickTop="1">
       <c r="A41" s="215" t="s">
         <v>97</v>
       </c>
@@ -19309,7 +19308,7 @@
       <c r="Y41" s="232"/>
       <c r="Z41" s="233"/>
       <c r="AA41" s="237" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="AB41" s="216"/>
       <c r="AC41" s="216"/>
@@ -19338,7 +19337,7 @@
       <c r="AV41" s="269"/>
       <c r="AW41" s="270"/>
     </row>
-    <row r="42" spans="1:49" s="19" customFormat="1" ht="17" customHeight="1">
+    <row r="42" spans="1:49" s="19" customFormat="1" ht="16.95" customHeight="1">
       <c r="A42" s="218"/>
       <c r="B42" s="219"/>
       <c r="C42" s="219"/>
@@ -19393,7 +19392,7 @@
       <c r="AV42" s="266"/>
       <c r="AW42" s="267"/>
     </row>
-    <row r="43" spans="1:49" ht="17" customHeight="1" thickBot="1">
+    <row r="43" spans="1:49" ht="16.95" customHeight="1" thickBot="1">
       <c r="A43" s="221"/>
       <c r="B43" s="222"/>
       <c r="C43" s="222"/>
@@ -19423,7 +19422,7 @@
       <c r="Y43" s="229"/>
       <c r="Z43" s="230"/>
       <c r="AA43" s="225" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="AB43" s="226"/>
       <c r="AC43" s="226"/>
@@ -19439,7 +19438,7 @@
       <c r="AK43" s="254"/>
       <c r="AL43" s="255"/>
       <c r="AM43" s="225" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="AN43" s="226"/>
       <c r="AO43" s="226"/>
@@ -21312,7 +21311,7 @@
       <c r="AV80" s="26"/>
       <c r="AW80" s="183"/>
     </row>
-    <row r="81" spans="1:50" s="19" customFormat="1" ht="23" customHeight="1" thickTop="1">
+    <row r="81" spans="1:50" s="19" customFormat="1" ht="22.95" customHeight="1" thickTop="1">
       <c r="A81" s="215" t="s">
         <v>97</v>
       </c>
@@ -21348,7 +21347,7 @@
       <c r="Y81" s="232"/>
       <c r="Z81" s="233"/>
       <c r="AA81" s="237" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="AB81" s="216"/>
       <c r="AC81" s="216"/>
@@ -21377,7 +21376,7 @@
       <c r="AV81" s="269"/>
       <c r="AW81" s="270"/>
     </row>
-    <row r="82" spans="1:50" s="19" customFormat="1" ht="23" customHeight="1">
+    <row r="82" spans="1:50" s="19" customFormat="1" ht="22.95" customHeight="1">
       <c r="A82" s="218"/>
       <c r="B82" s="219"/>
       <c r="C82" s="219"/>
@@ -21432,7 +21431,7 @@
       <c r="AV82" s="266"/>
       <c r="AW82" s="267"/>
     </row>
-    <row r="83" spans="1:50" ht="23" customHeight="1" thickBot="1">
+    <row r="83" spans="1:50" ht="22.95" customHeight="1" thickBot="1">
       <c r="A83" s="221"/>
       <c r="B83" s="222"/>
       <c r="C83" s="222"/>
@@ -21462,7 +21461,7 @@
       <c r="Y83" s="229"/>
       <c r="Z83" s="230"/>
       <c r="AA83" s="225" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="AB83" s="226"/>
       <c r="AC83" s="226"/>
@@ -23394,7 +23393,7 @@
       <c r="Y121" s="232"/>
       <c r="Z121" s="233"/>
       <c r="AA121" s="237" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="AB121" s="216"/>
       <c r="AC121" s="216"/>
@@ -23508,7 +23507,7 @@
       <c r="Y123" s="229"/>
       <c r="Z123" s="230"/>
       <c r="AA123" s="225" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="AB123" s="226"/>
       <c r="AC123" s="226"/>
@@ -24740,7 +24739,7 @@
       <c r="J147" s="51"/>
       <c r="K147" s="52"/>
       <c r="L147" s="53" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="M147" s="51"/>
       <c r="N147" s="51"/>
@@ -25681,15 +25680,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:BJ174"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A45" zoomScale="115" zoomScaleNormal="70" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="AT1" sqref="AT1:AW1"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A151" zoomScale="115" zoomScaleNormal="70" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="AH174" sqref="AH174"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="13.5" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="13.5" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.6640625" style="19" customWidth="1"/>
     <col min="2" max="2" width="2.6640625" style="28" customWidth="1"/>
@@ -25926,7 +25925,7 @@
       <c r="AU4" s="23"/>
       <c r="AW4" s="178"/>
     </row>
-    <row r="5" spans="1:58" ht="14">
+    <row r="5" spans="1:58" ht="13.8">
       <c r="A5" s="21"/>
       <c r="B5" s="28" t="s">
         <v>62</v>
@@ -26662,7 +26661,7 @@
       <c r="N41" s="216"/>
       <c r="O41" s="217"/>
       <c r="P41" s="224" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="Q41" s="216"/>
       <c r="R41" s="216"/>
@@ -26677,7 +26676,7 @@
       <c r="Y41" s="232"/>
       <c r="Z41" s="233"/>
       <c r="AA41" s="237" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="AB41" s="216"/>
       <c r="AC41" s="216"/>
@@ -26791,7 +26790,7 @@
       <c r="Y43" s="229"/>
       <c r="Z43" s="230"/>
       <c r="AA43" s="225" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="AB43" s="226"/>
       <c r="AC43" s="226"/>
@@ -26948,7 +26947,7 @@
         <v>1</v>
       </c>
       <c r="D49" s="82" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E49" s="83"/>
       <c r="F49" s="83"/>
@@ -26956,7 +26955,7 @@
       <c r="H49" s="84"/>
       <c r="I49" s="85"/>
       <c r="J49" s="86" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="K49" s="84"/>
       <c r="L49" s="84"/>
@@ -26976,7 +26975,7 @@
       </c>
       <c r="U49" s="89"/>
       <c r="V49" s="82" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="W49" s="83"/>
       <c r="X49" s="83"/>
@@ -27021,7 +27020,7 @@
       <c r="H50" s="95"/>
       <c r="I50" s="96"/>
       <c r="J50" s="97" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="K50" s="95"/>
       <c r="L50" s="95"/>
@@ -27041,7 +27040,7 @@
       </c>
       <c r="U50" s="101"/>
       <c r="V50" s="93" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="W50" s="94"/>
       <c r="X50" s="94"/>
@@ -27370,7 +27369,7 @@
       <c r="L57" s="167"/>
       <c r="M57" s="168"/>
       <c r="N57" s="166" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="O57" s="167"/>
       <c r="P57" s="167"/>
@@ -27415,7 +27414,7 @@
         <v>3</v>
       </c>
       <c r="D58" s="192" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E58" s="193"/>
       <c r="F58" s="193"/>
@@ -27427,7 +27426,7 @@
       <c r="L58" s="193"/>
       <c r="M58" s="194"/>
       <c r="N58" s="130" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="O58" s="128"/>
       <c r="P58" s="128"/>
@@ -28601,7 +28600,7 @@
       <c r="Y81" s="232"/>
       <c r="Z81" s="233"/>
       <c r="AA81" s="237" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="AB81" s="216"/>
       <c r="AC81" s="216"/>
@@ -28715,7 +28714,7 @@
       <c r="Y83" s="229"/>
       <c r="Z83" s="230"/>
       <c r="AA83" s="225" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="AB83" s="226"/>
       <c r="AC83" s="226"/>
@@ -28922,7 +28921,7 @@
     <row r="90" spans="1:49" ht="13.5" customHeight="1">
       <c r="A90" s="21"/>
       <c r="D90" s="23" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E90" s="23"/>
       <c r="F90" s="23"/>
@@ -28954,7 +28953,7 @@
     <row r="91" spans="1:49" ht="13.5" customHeight="1">
       <c r="A91" s="21"/>
       <c r="D91" s="23" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E91" s="23"/>
       <c r="F91" s="23"/>
@@ -29141,7 +29140,7 @@
     <row r="97" spans="1:49" ht="13.5" customHeight="1">
       <c r="A97" s="21"/>
       <c r="C97" s="19" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D97" s="23"/>
       <c r="E97" s="23"/>
@@ -29897,7 +29896,7 @@
       <c r="Y121" s="232"/>
       <c r="Z121" s="233"/>
       <c r="AA121" s="237" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="AB121" s="216"/>
       <c r="AC121" s="216"/>
@@ -30011,7 +30010,7 @@
       <c r="Y123" s="229"/>
       <c r="Z123" s="230"/>
       <c r="AA123" s="225" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="AB123" s="226"/>
       <c r="AC123" s="226"/>
@@ -30275,7 +30274,7 @@
         <v>1</v>
       </c>
       <c r="F131" s="123" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="G131" s="121"/>
       <c r="H131" s="121"/>
@@ -30285,7 +30284,7 @@
       <c r="L131" s="121"/>
       <c r="M131" s="122"/>
       <c r="N131" s="121" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="O131" s="121"/>
       <c r="P131" s="121"/>
@@ -30649,7 +30648,7 @@
         <v>3</v>
       </c>
       <c r="F138" s="128" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="G138" s="128"/>
       <c r="H138" s="128"/>
@@ -30659,7 +30658,7 @@
       <c r="L138" s="128"/>
       <c r="M138" s="128"/>
       <c r="N138" s="130" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="O138" s="128"/>
       <c r="P138" s="128"/>
@@ -31066,7 +31065,7 @@
         <v>1</v>
       </c>
       <c r="F146" s="155" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="G146" s="156"/>
       <c r="H146" s="156"/>
@@ -31100,7 +31099,7 @@
       <c r="AH146" s="159"/>
       <c r="AI146" s="164"/>
       <c r="AJ146" s="195" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="AK146" s="160"/>
       <c r="AL146" s="160"/>
@@ -31158,7 +31157,7 @@
       <c r="AH147" s="152"/>
       <c r="AI147" s="165"/>
       <c r="AJ147" s="196" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="AK147" s="153"/>
       <c r="AL147" s="153"/>
@@ -31182,7 +31181,7 @@
         <v>3</v>
       </c>
       <c r="F148" s="148" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="G148" s="149"/>
       <c r="H148" s="149"/>
@@ -31192,7 +31191,7 @@
       <c r="L148" s="150"/>
       <c r="M148" s="151"/>
       <c r="N148" s="148" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="O148" s="149"/>
       <c r="P148" s="149"/>
@@ -31216,7 +31215,7 @@
       <c r="AH148" s="152"/>
       <c r="AI148" s="165"/>
       <c r="AJ148" s="196" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="AK148" s="153"/>
       <c r="AL148" s="153"/>
@@ -31233,7 +31232,7 @@
       <c r="AW148" s="178"/>
       <c r="AY148" s="190"/>
     </row>
-    <row r="149" spans="1:62" ht="29" customHeight="1">
+    <row r="149" spans="1:62" ht="28.95" customHeight="1">
       <c r="A149" s="21"/>
       <c r="D149" s="23"/>
       <c r="E149" s="197">
@@ -31250,7 +31249,7 @@
       <c r="L149" s="175"/>
       <c r="M149" s="200"/>
       <c r="N149" s="361" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="O149" s="362"/>
       <c r="P149" s="362"/>
@@ -31274,7 +31273,7 @@
       <c r="AH149" s="362"/>
       <c r="AI149" s="363"/>
       <c r="AJ149" s="201" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="AK149" s="202"/>
       <c r="AL149" s="202"/>
@@ -31706,7 +31705,7 @@
       <c r="A158" s="21"/>
       <c r="D158" s="23"/>
       <c r="E158" s="141" t="s">
-        <v>109</v>
+        <v>143</v>
       </c>
       <c r="F158" s="132"/>
       <c r="G158" s="23"/>
@@ -31758,7 +31757,7 @@
       <c r="D159" s="142"/>
       <c r="E159" s="139"/>
       <c r="F159" s="12" t="s">
-        <v>110</v>
+        <v>144</v>
       </c>
       <c r="G159" s="12"/>
       <c r="H159" s="12"/>
@@ -31809,7 +31808,7 @@
       <c r="D160" s="142"/>
       <c r="E160" s="142"/>
       <c r="F160" s="206" t="s">
-        <v>111</v>
+        <v>145</v>
       </c>
       <c r="G160" s="12"/>
       <c r="H160" s="12"/>
@@ -31860,7 +31859,7 @@
       <c r="D161" s="142"/>
       <c r="E161" s="139"/>
       <c r="F161" s="206" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G161" s="12"/>
       <c r="H161" s="12"/>
@@ -31910,13 +31909,13 @@
       <c r="A162" s="21"/>
       <c r="D162" s="142"/>
       <c r="E162" s="207" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F162" s="204"/>
       <c r="G162" s="204"/>
       <c r="H162" s="205"/>
       <c r="I162" s="352" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="J162" s="353"/>
       <c r="K162" s="353"/>
@@ -31945,7 +31944,7 @@
       <c r="AH162" s="353"/>
       <c r="AI162" s="354"/>
       <c r="AJ162" s="352" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="AK162" s="353"/>
       <c r="AL162" s="353"/>
@@ -31965,13 +31964,13 @@
       <c r="A163" s="21"/>
       <c r="D163" s="142"/>
       <c r="E163" s="355" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F163" s="356"/>
       <c r="G163" s="356"/>
       <c r="H163" s="357"/>
       <c r="I163" s="208" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="J163" s="209"/>
       <c r="K163" s="209"/>
@@ -32000,7 +31999,7 @@
       <c r="AH163" s="209"/>
       <c r="AI163" s="211"/>
       <c r="AJ163" s="195" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="AK163" s="209"/>
       <c r="AL163" s="209"/>
@@ -32020,13 +32019,13 @@
       <c r="A164" s="21"/>
       <c r="D164" s="142"/>
       <c r="E164" s="358" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F164" s="359"/>
       <c r="G164" s="359"/>
       <c r="H164" s="360"/>
       <c r="I164" s="212" t="s">
-        <v>120</v>
+        <v>146</v>
       </c>
       <c r="J164" s="187"/>
       <c r="K164" s="187"/>
@@ -32055,7 +32054,7 @@
       <c r="AH164" s="187"/>
       <c r="AI164" s="189"/>
       <c r="AJ164" s="213" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="AK164" s="187"/>
       <c r="AL164" s="187"/>
@@ -32175,7 +32174,7 @@
     <row r="167" spans="1:50" ht="13.5" customHeight="1">
       <c r="A167" s="21"/>
       <c r="D167" s="142" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E167" s="12"/>
       <c r="F167" s="12"/>
@@ -32226,7 +32225,7 @@
     <row r="168" spans="1:50" ht="13.5" customHeight="1">
       <c r="A168" s="21"/>
       <c r="C168" s="19" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D168" s="142"/>
       <c r="E168" s="12"/>
@@ -32278,7 +32277,7 @@
     <row r="169" spans="1:50" ht="13.5" customHeight="1">
       <c r="A169" s="21"/>
       <c r="D169" s="142" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="E169" s="12"/>
       <c r="F169" s="12"/>
@@ -32329,7 +32328,7 @@
     <row r="170" spans="1:50" ht="13.5" customHeight="1">
       <c r="A170" s="21"/>
       <c r="D170" s="142" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E170" s="12"/>
       <c r="F170" s="12"/>
@@ -32660,7 +32659,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:AW684"/>
   <sheetViews>
@@ -32668,7 +32667,7 @@
       <selection sqref="A1:I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="13.2"/>
   <sheetData>
     <row r="1" spans="1:49" s="1" customFormat="1" ht="13.5" customHeight="1">
       <c r="A1" s="374"/>
@@ -35512,9 +35511,9 @@
               </from>
               <to>
                 <xdr:col>8</xdr:col>
-                <xdr:colOff>101600</xdr:colOff>
+                <xdr:colOff>99060</xdr:colOff>
                 <xdr:row>1</xdr:row>
-                <xdr:rowOff>165100</xdr:rowOff>
+                <xdr:rowOff>167640</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>

</xml_diff>